<commit_message>
Remove test data and replace with script that generates the test data
</commit_message>
<xml_diff>
--- a/python/extras/scripts/io_regression_test/Generic ETL Test 1.xlsx
+++ b/python/extras/scripts/io_regression_test/Generic ETL Test 1.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="108">
   <si>
     <t>PROJ: Generic Testing</t>
   </si>
@@ -34,6 +34,9 @@
     <t>PARAM</t>
   </si>
   <si>
+    <t>FILES</t>
+  </si>
+  <si>
     <t>MEAS</t>
   </si>
   <si>
@@ -127,48 +130,129 @@
     <t>Sample 1</t>
   </si>
   <si>
+    <t>results/DataFile01.txt</t>
+  </si>
+  <si>
+    <t>DataFile01.txt</t>
+  </si>
+  <si>
     <t>x</t>
   </si>
   <si>
     <t>Sample 2</t>
   </si>
   <si>
+    <t>results/DataFile02.txt</t>
+  </si>
+  <si>
+    <t>DataFile02.txt</t>
+  </si>
+  <si>
     <t>Sample 3</t>
   </si>
   <si>
+    <t>results/DataFile03.txt</t>
+  </si>
+  <si>
+    <t>DataFile03.txt</t>
+  </si>
+  <si>
     <t>Sample 4</t>
   </si>
   <si>
+    <t>results/DataFile04.txt</t>
+  </si>
+  <si>
+    <t>DataFile04.txt</t>
+  </si>
+  <si>
     <t>Sample 5</t>
   </si>
   <si>
+    <t>DataFile05.txt</t>
+  </si>
+  <si>
+    <t>DataFile06.txt</t>
+  </si>
+  <si>
+    <t>Otherdir, Subdir</t>
+  </si>
+  <si>
     <t>Sample 8</t>
   </si>
   <si>
+    <t>results/DataFile08.txt</t>
+  </si>
+  <si>
+    <t>file1.txt</t>
+  </si>
+  <si>
     <t>Sample 9</t>
   </si>
   <si>
+    <t>results/DataFile09.txt</t>
+  </si>
+  <si>
+    <t>Otherdir, results/DataFile03.txt, Subdir</t>
+  </si>
+  <si>
     <t>Sample 10</t>
   </si>
   <si>
+    <t>results/DataFile10.txt</t>
+  </si>
+  <si>
+    <t>DataFile10.txt</t>
+  </si>
+  <si>
     <t>Sample 11</t>
   </si>
   <si>
+    <t>DataFile11.txt</t>
+  </si>
+  <si>
+    <t>DataFile12.txt</t>
+  </si>
+  <si>
     <t>Sample 13</t>
   </si>
   <si>
+    <t>results/DataFile13.txt</t>
+  </si>
+  <si>
+    <t>DataFile13.txt</t>
+  </si>
+  <si>
     <t>Sample 14</t>
   </si>
   <si>
+    <t>results/DataFile14.txt</t>
+  </si>
+  <si>
+    <t>DataFile14.txt</t>
+  </si>
+  <si>
     <t>Sample 15</t>
   </si>
   <si>
+    <t>results/DataFile15.txt</t>
+  </si>
+  <si>
     <t>Sample 16</t>
   </si>
   <si>
+    <t>results/DataFile16.txt</t>
+  </si>
+  <si>
     <t>Sample 17</t>
   </si>
   <si>
+    <t>DataFile18.txt</t>
+  </si>
+  <si>
+    <t>DataFile19.txt</t>
+  </si>
+  <si>
     <t>Sample 20</t>
   </si>
   <si>
@@ -184,15 +268,27 @@
     <t>Sample 24</t>
   </si>
   <si>
+    <t>results/DataFile05.txt</t>
+  </si>
+  <si>
     <t>Sample 25</t>
   </si>
   <si>
+    <t>results/DataFile06.txt</t>
+  </si>
+  <si>
     <t>Sample 26</t>
   </si>
   <si>
+    <t>results/DataFile07.txt</t>
+  </si>
+  <si>
     <t>Sample 27</t>
   </si>
   <si>
+    <t>DataFile08.txt</t>
+  </si>
+  <si>
     <t>Sample 28</t>
   </si>
   <si>
@@ -202,9 +298,15 @@
     <t>Sample 30</t>
   </si>
   <si>
+    <t>results/DataFile11.txt</t>
+  </si>
+  <si>
     <t>Sample 31</t>
   </si>
   <si>
+    <t>results/DataFile12.txt</t>
+  </si>
+  <si>
     <t>Sample 32</t>
   </si>
   <si>
@@ -220,10 +322,19 @@
     <t>Sample 36</t>
   </si>
   <si>
+    <t>results/DataFile17.txt</t>
+  </si>
+  <si>
     <t>Sample 37</t>
   </si>
   <si>
+    <t>results/DataFile18.txt</t>
+  </si>
+  <si>
     <t>Sample 38</t>
+  </si>
+  <si>
+    <t>results/DataFile19.txt</t>
   </si>
 </sst>
 </file>
@@ -233,7 +344,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mmm d, yyyy"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -251,6 +362,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font/>
   </fonts>
   <fills count="3">
     <fill>
@@ -275,7 +387,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -321,10 +433,19 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -346,7 +467,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="37.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -364,16 +485,19 @@
         <v>2</v>
       </c>
       <c r="I1" s="4"/>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="3"/>
+      <c r="K1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="4"/>
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
       <c r="N1" s="4"/>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
@@ -403,8 +527,8 @@
       <c r="I2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>6</v>
+      <c r="J2" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>6</v>
@@ -419,43 +543,48 @@
         <v>6</v>
       </c>
       <c r="O2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="R2" s="3"/>
+      <c r="S2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="P2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" ht="37.5">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="I3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="J3" s="1"/>
+      <c r="K3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L3" s="3" t="s">
@@ -470,27 +599,32 @@
       <c r="O3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="P3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="Q3" s="1" t="s">
         <v>20</v>
+      </c>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="7"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
@@ -500,40 +634,41 @@
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
-      <c r="Q4" s="4"/>
-    </row>
-    <row r="5">
+      <c r="Q4" s="3"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+    </row>
+    <row r="5" ht="62.25">
       <c r="A5" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G5" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="9" t="s">
-        <v>29</v>
-      </c>
       <c r="I5" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="K5" s="10" t="s">
+      <c r="J5" s="9"/>
+      <c r="K5" s="9" t="s">
         <v>32</v>
       </c>
       <c r="L5" s="10" t="s">
@@ -542,19 +677,24 @@
       <c r="M5" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="N5" s="9" t="s">
+      <c r="N5" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="O5" s="9"/>
+      <c r="O5" s="9" t="s">
+        <v>36</v>
+      </c>
       <c r="P5" s="9"/>
       <c r="Q5" s="9"/>
-    </row>
-    <row r="6">
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="9"/>
+    </row>
+    <row r="6" ht="18.75">
       <c r="A6" s="11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C6" s="13">
         <v>1001.0</v>
@@ -577,34 +717,43 @@
       <c r="I6" s="14">
         <v>2.7</v>
       </c>
-      <c r="J6" s="15">
+      <c r="J6" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="K6" s="16">
         <v>5.0</v>
       </c>
-      <c r="K6" s="16">
+      <c r="L6" s="17">
         <v>42736.0</v>
       </c>
-      <c r="L6" s="14">
+      <c r="M6" s="14">
         <v>400.0</v>
       </c>
-      <c r="M6" s="14">
+      <c r="N6" s="14">
         <v>300.0</v>
       </c>
-      <c r="N6" s="14">
+      <c r="O6" s="14">
         <v>194.0</v>
       </c>
-      <c r="O6" s="13">
+      <c r="P6" s="13">
         <v>46.0</v>
       </c>
-      <c r="P6" s="13">
+      <c r="Q6" s="13">
         <v>1890.0</v>
       </c>
-      <c r="Q6" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7">
+      <c r="R6" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="S6" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="T6" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" ht="18.75">
       <c r="B7" s="12" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C7" s="13">
         <v>1002.0</v>
@@ -627,34 +776,43 @@
       <c r="I7" s="14">
         <v>8.200000000000001</v>
       </c>
-      <c r="J7" s="15">
+      <c r="J7" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="K7" s="16">
         <v>8.0</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>42737.0</v>
       </c>
-      <c r="L7" s="14">
+      <c r="M7" s="14">
         <v>1700.0</v>
       </c>
-      <c r="M7" s="14">
+      <c r="N7" s="14">
         <v>500.0</v>
       </c>
-      <c r="N7" s="14">
+      <c r="O7" s="14">
         <v>186.0</v>
       </c>
-      <c r="O7" s="13">
+      <c r="P7" s="13">
         <v>75.0</v>
       </c>
-      <c r="P7" s="13">
+      <c r="Q7" s="13">
         <v>710.0</v>
       </c>
-      <c r="Q7" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8">
+      <c r="R7" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="S7" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="T7" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" ht="18.75">
       <c r="B8" s="12" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C8" s="13">
         <v>1003.0</v>
@@ -677,34 +835,43 @@
       <c r="I8" s="14">
         <v>3.8000000000000003</v>
       </c>
-      <c r="J8" s="15">
+      <c r="J8" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="K8" s="16">
         <v>1.0</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>42738.0</v>
       </c>
-      <c r="L8" s="14">
+      <c r="M8" s="14">
         <v>1600.0</v>
       </c>
-      <c r="M8" s="14">
+      <c r="N8" s="14">
         <v>500.0</v>
       </c>
-      <c r="N8" s="14">
+      <c r="O8" s="14">
         <v>81.0</v>
       </c>
-      <c r="O8" s="13">
+      <c r="P8" s="13">
         <v>57.0</v>
       </c>
-      <c r="P8" s="13">
+      <c r="Q8" s="13">
         <v>670.0</v>
       </c>
-      <c r="Q8" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9">
+      <c r="R8" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="S8" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="T8" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" ht="18.75">
       <c r="B9" s="12" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C9" s="13">
         <v>1004.0</v>
@@ -727,32 +894,38 @@
       <c r="I9" s="14">
         <v>8.0</v>
       </c>
-      <c r="J9" s="15">
+      <c r="J9" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="K9" s="16">
         <v>3.0</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>42739.0</v>
       </c>
-      <c r="L9" s="14">
+      <c r="M9" s="14">
         <v>900.0</v>
       </c>
-      <c r="M9" s="14">
+      <c r="N9" s="14">
         <v>300.0</v>
       </c>
-      <c r="N9" s="14">
+      <c r="O9" s="14">
         <v>104.00000000000001</v>
       </c>
-      <c r="O9" s="13">
+      <c r="P9" s="13">
         <v>31.0</v>
       </c>
-      <c r="P9" s="13">
+      <c r="Q9" s="13">
         <v>1920.0</v>
       </c>
-      <c r="Q9" s="15"/>
-    </row>
-    <row r="10">
+      <c r="R9" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="T9" s="16"/>
+    </row>
+    <row r="10" ht="18.75">
       <c r="B10" s="12" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="C10" s="13">
         <v>1005.0</v>
@@ -775,32 +948,37 @@
       <c r="I10" s="14">
         <v>5.300000000000001</v>
       </c>
-      <c r="J10" s="15">
+      <c r="J10" s="15"/>
+      <c r="K10" s="16">
         <v>1.0</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>42740.0</v>
       </c>
-      <c r="L10" s="14">
+      <c r="M10" s="14">
         <v>2200.0</v>
       </c>
-      <c r="M10" s="14">
+      <c r="N10" s="14">
         <v>300.0</v>
       </c>
-      <c r="N10" s="14">
+      <c r="O10" s="14">
         <v>54.00000000000001</v>
       </c>
-      <c r="O10" s="13">
+      <c r="P10" s="13">
         <v>72.0</v>
       </c>
-      <c r="P10" s="13">
+      <c r="Q10" s="13">
         <v>1900.0</v>
       </c>
-      <c r="Q10" s="15"/>
-    </row>
-    <row r="11">
+      <c r="R10" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="S10" s="18"/>
+      <c r="T10" s="16"/>
+    </row>
+    <row r="11" ht="18.75">
       <c r="B11" s="12" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="C11" s="13">
         <v>1005.0</v>
@@ -823,34 +1001,41 @@
       <c r="I11" s="14">
         <v>5.300000000000001</v>
       </c>
-      <c r="J11" s="15">
+      <c r="J11" s="15"/>
+      <c r="K11" s="16">
         <v>7.0</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>42741.0</v>
       </c>
-      <c r="L11" s="14">
+      <c r="M11" s="14">
         <v>2200.0</v>
       </c>
-      <c r="M11" s="14">
+      <c r="N11" s="14">
         <v>100.0</v>
       </c>
-      <c r="N11" s="14">
+      <c r="O11" s="14">
         <v>51.0</v>
       </c>
-      <c r="O11" s="13">
+      <c r="P11" s="13">
         <v>48.0</v>
       </c>
-      <c r="P11" s="13">
+      <c r="Q11" s="13">
         <v>1130.0</v>
       </c>
-      <c r="Q11" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12">
+      <c r="R11" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="S11" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="T11" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" ht="18.75">
       <c r="B12" s="12" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="C12" s="13">
         <v>1005.0</v>
@@ -873,32 +1058,37 @@
       <c r="I12" s="14">
         <v>5.300000000000001</v>
       </c>
-      <c r="J12" s="15">
+      <c r="J12" s="15"/>
+      <c r="K12" s="16">
         <v>8.0</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>42742.0</v>
       </c>
-      <c r="L12" s="14">
+      <c r="M12" s="14">
         <v>700.0</v>
       </c>
-      <c r="M12" s="14">
+      <c r="N12" s="14">
         <v>200.0</v>
       </c>
-      <c r="N12" s="14">
+      <c r="O12" s="14">
         <v>35.0</v>
       </c>
-      <c r="O12" s="13">
+      <c r="P12" s="13">
         <v>62.0</v>
       </c>
-      <c r="P12" s="13">
+      <c r="Q12" s="13">
         <v>1140.0</v>
       </c>
-      <c r="Q12" s="15"/>
-    </row>
-    <row r="13">
+      <c r="R12" s="15"/>
+      <c r="S12" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="T12" s="16"/>
+    </row>
+    <row r="13" ht="18.75">
       <c r="B13" s="12" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="C13" s="13">
         <v>1008.0</v>
@@ -921,32 +1111,39 @@
       <c r="I13" s="14">
         <v>9.3</v>
       </c>
-      <c r="J13" s="15">
+      <c r="J13" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="K13" s="16">
         <v>4.0</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>42743.0</v>
       </c>
-      <c r="L13" s="14">
+      <c r="M13" s="14">
         <v>1500.0</v>
       </c>
-      <c r="M13" s="14">
+      <c r="N13" s="14">
         <v>500.0</v>
       </c>
-      <c r="N13" s="14">
+      <c r="O13" s="14">
         <v>60.0</v>
       </c>
-      <c r="O13" s="13">
+      <c r="P13" s="13">
         <v>49.0</v>
       </c>
-      <c r="P13" s="13">
+      <c r="Q13" s="13">
         <v>100.0</v>
       </c>
-      <c r="Q13" s="15"/>
-    </row>
-    <row r="14">
+      <c r="R13" s="15"/>
+      <c r="S13" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="T13" s="16"/>
+    </row>
+    <row r="14" ht="18.75">
       <c r="B14" s="12" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="C14" s="13">
         <v>1009.0</v>
@@ -969,32 +1166,39 @@
       <c r="I14" s="14">
         <v>3.0</v>
       </c>
-      <c r="J14" s="15">
+      <c r="J14" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="K14" s="16">
         <v>7.0</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>42744.0</v>
       </c>
-      <c r="L14" s="14">
+      <c r="M14" s="14">
         <v>1400.0</v>
       </c>
-      <c r="M14" s="14">
+      <c r="N14" s="14">
         <v>500.0</v>
       </c>
-      <c r="N14" s="14">
+      <c r="O14" s="14">
         <v>76.0</v>
       </c>
-      <c r="O14" s="13">
+      <c r="P14" s="13">
         <v>34.0</v>
       </c>
-      <c r="P14" s="13">
+      <c r="Q14" s="13">
         <v>520.0</v>
       </c>
-      <c r="Q14" s="15"/>
-    </row>
-    <row r="15">
+      <c r="R14" s="15"/>
+      <c r="S14" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="T14" s="16"/>
+    </row>
+    <row r="15" ht="18.75">
       <c r="B15" s="12" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="C15" s="13">
         <v>1010.0</v>
@@ -1013,34 +1217,43 @@
       <c r="I15" s="14">
         <v>10.9</v>
       </c>
-      <c r="J15" s="15">
+      <c r="J15" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="K15" s="16">
         <v>3.0</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <v>42745.0</v>
       </c>
-      <c r="L15" s="14">
+      <c r="M15" s="14">
         <v>900.0</v>
       </c>
-      <c r="M15" s="14">
+      <c r="N15" s="14">
         <v>200.0</v>
       </c>
-      <c r="N15" s="14">
+      <c r="O15" s="14">
         <v>54.00000000000001</v>
       </c>
-      <c r="O15" s="13">
+      <c r="P15" s="13">
         <v>38.0</v>
       </c>
-      <c r="P15" s="13">
+      <c r="Q15" s="13">
         <v>1270.0</v>
       </c>
-      <c r="Q15" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16">
+      <c r="R15" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="S15" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="T15" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" ht="18.75">
       <c r="B16" s="12" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="C16" s="13">
         <v>1011.0</v>
@@ -1059,34 +1272,41 @@
       <c r="I16" s="14">
         <v>4.0</v>
       </c>
-      <c r="J16" s="15">
+      <c r="J16" s="15"/>
+      <c r="K16" s="16">
         <v>4.0</v>
       </c>
-      <c r="K16">
+      <c r="L16">
         <v>42746.0</v>
       </c>
-      <c r="L16" s="14">
+      <c r="M16" s="14">
         <v>1700.0</v>
       </c>
-      <c r="M16" s="14">
+      <c r="N16" s="14">
         <v>500.0</v>
       </c>
-      <c r="N16" s="14">
+      <c r="O16" s="14">
         <v>52.0</v>
       </c>
-      <c r="O16" s="13">
+      <c r="P16" s="13">
         <v>48.0</v>
       </c>
-      <c r="P16" s="13">
+      <c r="Q16" s="13">
         <v>970.0</v>
       </c>
-      <c r="Q16" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17">
+      <c r="R16" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="S16" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="T16" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" ht="18.75">
       <c r="B17" s="12" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="C17" s="13">
         <v>1011.0</v>
@@ -1105,34 +1325,41 @@
       <c r="I17" s="14">
         <v>4.0</v>
       </c>
-      <c r="J17" s="15">
+      <c r="J17" s="15"/>
+      <c r="K17" s="16">
         <v>1.0</v>
       </c>
-      <c r="K17">
+      <c r="L17">
         <v>42747.0</v>
       </c>
-      <c r="L17" s="14">
+      <c r="M17" s="14">
         <v>800.0</v>
       </c>
-      <c r="M17" s="14">
+      <c r="N17" s="14">
         <v>200.0</v>
       </c>
-      <c r="N17" s="14">
+      <c r="O17" s="14">
         <v>74.0</v>
       </c>
-      <c r="O17" s="13">
+      <c r="P17" s="13">
         <v>59.0</v>
       </c>
-      <c r="P17" s="13">
+      <c r="Q17" s="13">
         <v>930.0</v>
       </c>
-      <c r="Q17" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18">
+      <c r="R17" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="S17" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="T17" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" ht="18.75">
       <c r="B18" s="12" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="C18" s="13">
         <v>1013.0</v>
@@ -1151,34 +1378,43 @@
       <c r="I18" s="14">
         <v>1.9000000000000001</v>
       </c>
-      <c r="J18" s="15">
+      <c r="J18" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="K18" s="16">
         <v>8.0</v>
       </c>
-      <c r="K18">
+      <c r="L18">
         <v>42748.0</v>
       </c>
-      <c r="L18" s="14">
+      <c r="M18" s="14">
         <v>1300.0</v>
       </c>
-      <c r="M18" s="14">
+      <c r="N18" s="14">
         <v>200.0</v>
       </c>
-      <c r="N18" s="14">
+      <c r="O18" s="14">
         <v>182.00000000000003</v>
       </c>
-      <c r="O18" s="13">
+      <c r="P18" s="13">
         <v>80.0</v>
       </c>
-      <c r="P18" s="13">
+      <c r="Q18" s="13">
         <v>230.0</v>
       </c>
-      <c r="Q18" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19">
+      <c r="R18" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="S18" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="T18" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" ht="18.75">
       <c r="B19" s="12" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="C19" s="13">
         <v>1014.0</v>
@@ -1197,34 +1433,43 @@
       <c r="I19" s="14">
         <v>10.3</v>
       </c>
-      <c r="J19" s="15">
+      <c r="J19" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="K19" s="16">
         <v>1.0</v>
       </c>
-      <c r="K19">
+      <c r="L19">
         <v>42749.0</v>
       </c>
-      <c r="L19" s="14">
+      <c r="M19" s="14">
         <v>1500.0</v>
       </c>
-      <c r="M19" s="14">
+      <c r="N19" s="14">
         <v>500.0</v>
       </c>
-      <c r="N19" s="14">
+      <c r="O19" s="14">
         <v>82.0</v>
       </c>
-      <c r="O19" s="13">
+      <c r="P19" s="13">
         <v>77.0</v>
       </c>
-      <c r="P19" s="13">
+      <c r="Q19" s="13">
         <v>1970.0</v>
       </c>
-      <c r="Q19" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20">
+      <c r="R19" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="S19" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="T19" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" ht="18.75">
       <c r="B20" s="12" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="C20" s="13">
         <v>1015.0</v>
@@ -1243,32 +1488,36 @@
       <c r="I20" s="14">
         <v>9.9</v>
       </c>
-      <c r="J20" s="15">
+      <c r="J20" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="K20" s="16">
         <v>10.0</v>
       </c>
-      <c r="K20">
+      <c r="L20">
         <v>42750.0</v>
       </c>
-      <c r="L20" s="14">
+      <c r="M20" s="14">
         <v>1100.0</v>
       </c>
-      <c r="M20" s="14">
+      <c r="N20" s="14">
         <v>100.0</v>
       </c>
-      <c r="N20" s="14">
+      <c r="O20" s="14">
         <v>117.0</v>
       </c>
-      <c r="O20" s="13">
+      <c r="P20" s="13">
         <v>84.0</v>
       </c>
-      <c r="P20" s="13">
+      <c r="Q20" s="13">
         <v>760.0</v>
       </c>
-      <c r="Q20" s="15"/>
-    </row>
-    <row r="21">
+      <c r="R20" s="15"/>
+      <c r="T20" s="16"/>
+    </row>
+    <row r="21" ht="18.75">
       <c r="B21" s="12" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="C21" s="13">
         <v>1016.0</v>
@@ -1287,32 +1536,36 @@
       <c r="I21" s="14">
         <v>9.600000000000001</v>
       </c>
-      <c r="J21" s="15">
+      <c r="J21" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="K21" s="16">
         <v>8.0</v>
       </c>
-      <c r="K21">
+      <c r="L21">
         <v>42751.0</v>
       </c>
-      <c r="L21" s="14">
+      <c r="M21" s="14">
         <v>900.0</v>
       </c>
-      <c r="M21" s="14">
+      <c r="N21" s="14">
         <v>300.0</v>
       </c>
-      <c r="N21" s="14">
+      <c r="O21" s="14">
         <v>174.0</v>
       </c>
-      <c r="O21" s="13">
+      <c r="P21" s="13">
         <v>94.0</v>
       </c>
-      <c r="P21" s="13">
+      <c r="Q21" s="13">
         <v>600.0</v>
       </c>
-      <c r="Q21" s="15"/>
-    </row>
-    <row r="22">
+      <c r="R21" s="15"/>
+      <c r="T21" s="16"/>
+    </row>
+    <row r="22" ht="18.75">
       <c r="B22" s="12" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="C22" s="13">
         <v>1017.0</v>
@@ -1331,32 +1584,35 @@
       </c>
       <c r="H22" s="13"/>
       <c r="I22" s="14"/>
-      <c r="J22" s="15">
+      <c r="J22" s="15"/>
+      <c r="K22" s="16">
         <v>5.0</v>
       </c>
-      <c r="K22">
+      <c r="L22">
         <v>42752.0</v>
       </c>
-      <c r="L22" s="14">
+      <c r="M22" s="14">
         <v>1300.0</v>
       </c>
-      <c r="M22" s="14">
+      <c r="N22" s="14">
         <v>200.0</v>
       </c>
-      <c r="N22" s="14">
+      <c r="O22" s="14">
         <v>99.0</v>
       </c>
-      <c r="O22" s="13">
+      <c r="P22" s="13">
         <v>84.0</v>
       </c>
-      <c r="P22" s="13">
+      <c r="Q22" s="13">
         <v>760.0</v>
       </c>
-      <c r="Q22" s="15"/>
-    </row>
-    <row r="23">
+      <c r="R22" s="15"/>
+      <c r="S22" s="18"/>
+      <c r="T22" s="16"/>
+    </row>
+    <row r="23" ht="18.75">
       <c r="B23" s="12" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="C23" s="13">
         <v>1017.0</v>
@@ -1375,34 +1631,41 @@
       </c>
       <c r="H23" s="13"/>
       <c r="I23" s="14"/>
-      <c r="J23" s="15">
+      <c r="J23" s="15"/>
+      <c r="K23" s="16">
         <v>1.0</v>
       </c>
-      <c r="K23">
+      <c r="L23">
         <v>42753.0</v>
       </c>
-      <c r="L23" s="14">
+      <c r="M23" s="14">
         <v>300.0</v>
       </c>
-      <c r="M23" s="14">
+      <c r="N23" s="14">
         <v>400.0</v>
       </c>
-      <c r="N23" s="14">
+      <c r="O23" s="14">
         <v>125.00000000000001</v>
       </c>
-      <c r="O23" s="13">
+      <c r="P23" s="13">
         <v>46.0</v>
       </c>
-      <c r="P23" s="13">
+      <c r="Q23" s="13">
         <v>1250.0</v>
       </c>
-      <c r="Q23" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24">
+      <c r="R23" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="S23" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="T23" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" ht="18.75">
       <c r="B24" s="12" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="C24" s="13">
         <v>1017.0</v>
@@ -1421,34 +1684,41 @@
       </c>
       <c r="H24" s="13"/>
       <c r="I24" s="14"/>
-      <c r="J24" s="15">
+      <c r="J24" s="15"/>
+      <c r="K24" s="16">
         <v>5.0</v>
       </c>
-      <c r="K24">
+      <c r="L24">
         <v>42754.0</v>
       </c>
-      <c r="L24" s="14">
+      <c r="M24" s="14">
         <v>800.0</v>
       </c>
-      <c r="M24" s="14">
+      <c r="N24" s="14">
         <v>500.0</v>
       </c>
-      <c r="N24" s="14">
+      <c r="O24" s="14">
         <v>165.0</v>
       </c>
-      <c r="O24" s="13">
+      <c r="P24" s="13">
         <v>43.0</v>
       </c>
-      <c r="P24" s="13">
+      <c r="Q24" s="13">
         <v>1050.0</v>
       </c>
-      <c r="Q24" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25">
+      <c r="R24" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="S24" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="T24" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" ht="18.75">
       <c r="B25" s="12" t="s">
-        <v>52</v>
+        <v>80</v>
       </c>
       <c r="C25" s="13">
         <v>1020.0</v>
@@ -1467,34 +1737,43 @@
       </c>
       <c r="H25" s="13"/>
       <c r="I25" s="14"/>
-      <c r="J25" s="15">
+      <c r="J25" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="K25" s="16">
         <v>10.0</v>
       </c>
-      <c r="K25">
+      <c r="L25">
         <v>42755.0</v>
       </c>
-      <c r="L25" s="14">
+      <c r="M25" s="14">
         <v>800.0</v>
       </c>
-      <c r="M25" s="14">
+      <c r="N25" s="14">
         <v>200.0</v>
       </c>
-      <c r="N25" s="14">
+      <c r="O25" s="14">
         <v>124.00000000000001</v>
       </c>
-      <c r="O25" s="13">
+      <c r="P25" s="13">
         <v>57.0</v>
       </c>
-      <c r="P25" s="13">
+      <c r="Q25" s="13">
         <v>410.0</v>
       </c>
-      <c r="Q25" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26">
+      <c r="R25" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="S25" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="T25" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" ht="18.75">
       <c r="B26" s="12" t="s">
-        <v>53</v>
+        <v>81</v>
       </c>
       <c r="C26" s="13">
         <v>1021.0</v>
@@ -1513,32 +1792,37 @@
       </c>
       <c r="H26" s="13"/>
       <c r="I26" s="14"/>
-      <c r="J26" s="15">
+      <c r="J26" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="K26" s="16">
         <v>9.0</v>
       </c>
-      <c r="K26">
+      <c r="L26">
         <v>42756.0</v>
       </c>
-      <c r="L26" s="14">
+      <c r="M26" s="14">
         <v>1500.0</v>
       </c>
-      <c r="M26" s="14">
+      <c r="N26" s="14">
         <v>300.0</v>
       </c>
-      <c r="N26" s="14">
+      <c r="O26" s="14">
         <v>83.0</v>
       </c>
-      <c r="O26" s="13">
+      <c r="P26" s="13">
         <v>48.0</v>
       </c>
-      <c r="P26" s="13">
+      <c r="Q26" s="13">
         <v>260.0</v>
       </c>
-      <c r="Q26" s="15"/>
-    </row>
-    <row r="27">
+      <c r="R26" s="15"/>
+      <c r="S26" s="18"/>
+      <c r="T26" s="16"/>
+    </row>
+    <row r="27" ht="18.75">
       <c r="B27" s="12" t="s">
-        <v>54</v>
+        <v>82</v>
       </c>
       <c r="C27" s="13">
         <v>1022.0</v>
@@ -1557,32 +1841,37 @@
       </c>
       <c r="H27" s="13"/>
       <c r="I27" s="14"/>
-      <c r="J27" s="15">
+      <c r="J27" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="K27" s="16">
         <v>6.0</v>
       </c>
-      <c r="K27">
+      <c r="L27">
         <v>42757.0</v>
       </c>
-      <c r="L27" s="14">
+      <c r="M27" s="14">
         <v>600.0</v>
       </c>
-      <c r="M27" s="14">
+      <c r="N27" s="14">
         <v>300.0</v>
       </c>
-      <c r="N27" s="14">
+      <c r="O27" s="14">
         <v>98.0</v>
       </c>
-      <c r="O27" s="13">
+      <c r="P27" s="13">
         <v>34.0</v>
       </c>
-      <c r="P27" s="13">
+      <c r="Q27" s="13">
         <v>2020.0</v>
       </c>
-      <c r="Q27" s="15"/>
-    </row>
-    <row r="28">
+      <c r="R27" s="15"/>
+      <c r="S27" s="18"/>
+      <c r="T27" s="16"/>
+    </row>
+    <row r="28" ht="18.75">
       <c r="B28" s="12" t="s">
-        <v>55</v>
+        <v>83</v>
       </c>
       <c r="C28" s="13">
         <v>1023.0</v>
@@ -1601,34 +1890,43 @@
       </c>
       <c r="H28" s="13"/>
       <c r="I28" s="14"/>
-      <c r="J28" s="15">
+      <c r="J28" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="K28" s="16">
         <v>6.0</v>
       </c>
-      <c r="K28">
+      <c r="L28">
         <v>42758.0</v>
       </c>
-      <c r="L28" s="14">
+      <c r="M28" s="14">
         <v>2200.0</v>
       </c>
-      <c r="M28" s="14">
+      <c r="N28" s="14">
         <v>500.0</v>
       </c>
-      <c r="N28" s="14">
+      <c r="O28" s="14">
         <v>58.0</v>
       </c>
-      <c r="O28" s="13">
+      <c r="P28" s="13">
         <v>80.0</v>
       </c>
-      <c r="P28" s="13">
+      <c r="Q28" s="13">
         <v>730.0</v>
       </c>
-      <c r="Q28" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="29">
+      <c r="R28" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="S28" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="T28" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" ht="18.75">
       <c r="B29" s="12" t="s">
-        <v>56</v>
+        <v>84</v>
       </c>
       <c r="C29" s="13">
         <v>1024.0</v>
@@ -1647,34 +1945,43 @@
       </c>
       <c r="H29" s="13"/>
       <c r="I29" s="14"/>
-      <c r="J29" s="15">
+      <c r="J29" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="K29" s="16">
         <v>10.0</v>
       </c>
-      <c r="K29">
+      <c r="L29">
         <v>42759.0</v>
       </c>
-      <c r="L29" s="14">
+      <c r="M29" s="14">
         <v>1300.0</v>
       </c>
-      <c r="M29" s="14">
+      <c r="N29" s="14">
         <v>200.0</v>
       </c>
-      <c r="N29" s="14">
+      <c r="O29" s="14">
         <v>193.0</v>
       </c>
-      <c r="O29" s="13">
+      <c r="P29" s="13">
         <v>33.0</v>
       </c>
-      <c r="P29" s="13">
+      <c r="Q29" s="13">
         <v>530.0</v>
       </c>
-      <c r="Q29" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="30">
+      <c r="R29" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="S29" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="T29" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" ht="18.75">
       <c r="B30" s="12" t="s">
-        <v>57</v>
+        <v>86</v>
       </c>
       <c r="C30" s="13">
         <v>1025.0</v>
@@ -1693,34 +2000,43 @@
       </c>
       <c r="H30" s="13"/>
       <c r="I30" s="14"/>
-      <c r="J30" s="15">
+      <c r="J30" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="K30" s="16">
         <v>9.0</v>
       </c>
-      <c r="K30">
+      <c r="L30">
         <v>42760.0</v>
       </c>
-      <c r="L30" s="14">
+      <c r="M30" s="14">
         <v>300.0</v>
       </c>
-      <c r="M30" s="14">
+      <c r="N30" s="14">
         <v>400.0</v>
       </c>
-      <c r="N30" s="14">
+      <c r="O30" s="14">
         <v>103.0</v>
       </c>
-      <c r="O30" s="13">
+      <c r="P30" s="13">
         <v>51.0</v>
       </c>
-      <c r="P30" s="13">
+      <c r="Q30" s="13">
         <v>1190.0</v>
       </c>
-      <c r="Q30" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="31">
+      <c r="R30" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="S30" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="T30" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" ht="18.75">
       <c r="B31" s="12" t="s">
-        <v>58</v>
+        <v>88</v>
       </c>
       <c r="C31" s="13">
         <v>1026.0</v>
@@ -1739,32 +2055,37 @@
       </c>
       <c r="H31" s="13"/>
       <c r="I31" s="14"/>
-      <c r="J31" s="15">
+      <c r="J31" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="K31" s="16">
         <v>10.0</v>
       </c>
-      <c r="K31">
+      <c r="L31">
         <v>42761.0</v>
       </c>
-      <c r="L31" s="14">
+      <c r="M31" s="14">
         <v>2200.0</v>
       </c>
-      <c r="M31" s="14">
+      <c r="N31" s="14">
         <v>100.0</v>
       </c>
-      <c r="N31" s="14">
+      <c r="O31" s="14">
         <v>80.0</v>
       </c>
-      <c r="O31" s="13">
+      <c r="P31" s="13">
         <v>77.0</v>
       </c>
-      <c r="P31" s="13">
+      <c r="Q31" s="13">
         <v>180.0</v>
       </c>
-      <c r="Q31" s="15"/>
-    </row>
-    <row r="32">
+      <c r="R31" s="15"/>
+      <c r="S31" s="18"/>
+      <c r="T31" s="16"/>
+    </row>
+    <row r="32" ht="18.75">
       <c r="B32" s="12" t="s">
-        <v>59</v>
+        <v>90</v>
       </c>
       <c r="C32" s="13">
         <v>1027.0</v>
@@ -1787,34 +2108,43 @@
       <c r="I32" s="14">
         <v>11.600000000000001</v>
       </c>
-      <c r="J32" s="15">
+      <c r="J32" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="K32" s="16">
         <v>6.0</v>
       </c>
-      <c r="K32">
+      <c r="L32">
         <v>42762.0</v>
       </c>
-      <c r="L32" s="14">
+      <c r="M32" s="14">
         <v>1700.0</v>
       </c>
-      <c r="M32" s="14">
+      <c r="N32" s="14">
         <v>200.0</v>
       </c>
-      <c r="N32" s="14">
+      <c r="O32" s="14">
         <v>186.0</v>
       </c>
-      <c r="O32" s="13">
+      <c r="P32" s="13">
         <v>56.0</v>
       </c>
-      <c r="P32" s="13">
+      <c r="Q32" s="13">
         <v>290.0</v>
       </c>
-      <c r="Q32" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="33">
+      <c r="R32" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="S32" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="T32" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" ht="18.75">
       <c r="B33" s="12" t="s">
-        <v>60</v>
+        <v>92</v>
       </c>
       <c r="C33" s="13">
         <v>1028.0</v>
@@ -1837,32 +2167,37 @@
       <c r="I33" s="14">
         <v>6.7</v>
       </c>
-      <c r="J33" s="15">
+      <c r="J33" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="K33" s="16">
         <v>7.0</v>
       </c>
-      <c r="K33">
+      <c r="L33">
         <v>42763.0</v>
       </c>
-      <c r="L33" s="14">
+      <c r="M33" s="14">
         <v>1400.0</v>
       </c>
-      <c r="M33" s="14">
+      <c r="N33" s="14">
         <v>300.0</v>
       </c>
-      <c r="N33" s="14">
+      <c r="O33" s="14">
         <v>162.0</v>
       </c>
-      <c r="O33" s="13">
+      <c r="P33" s="13">
         <v>37.0</v>
       </c>
-      <c r="P33" s="13">
+      <c r="Q33" s="13">
         <v>1200.0</v>
       </c>
-      <c r="Q33" s="15"/>
-    </row>
-    <row r="34">
+      <c r="R33" s="15"/>
+      <c r="S33" s="18"/>
+      <c r="T33" s="16"/>
+    </row>
+    <row r="34" ht="18.75">
       <c r="B34" s="12" t="s">
-        <v>61</v>
+        <v>93</v>
       </c>
       <c r="C34" s="13">
         <v>1029.0</v>
@@ -1885,32 +2220,37 @@
       <c r="I34" s="14">
         <v>11.5</v>
       </c>
-      <c r="J34" s="15">
+      <c r="J34" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="K34" s="16">
         <v>6.0</v>
       </c>
-      <c r="K34">
+      <c r="L34">
         <v>42764.0</v>
       </c>
-      <c r="L34" s="14">
+      <c r="M34" s="14">
         <v>1400.0</v>
       </c>
-      <c r="M34" s="14">
+      <c r="N34" s="14">
         <v>400.0</v>
       </c>
-      <c r="N34" s="14">
+      <c r="O34" s="14">
         <v>86.0</v>
       </c>
-      <c r="O34" s="13">
+      <c r="P34" s="13">
         <v>86.0</v>
       </c>
-      <c r="P34" s="13">
+      <c r="Q34" s="13">
         <v>100.0</v>
       </c>
-      <c r="Q34" s="15"/>
-    </row>
-    <row r="35">
+      <c r="R34" s="15"/>
+      <c r="S34" s="18"/>
+      <c r="T34" s="16"/>
+    </row>
+    <row r="35" ht="18.75">
       <c r="B35" s="12" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
       <c r="C35" s="13">
         <v>1030.0</v>
@@ -1933,32 +2273,37 @@
       <c r="I35" s="14">
         <v>8.3</v>
       </c>
-      <c r="J35" s="15">
+      <c r="J35" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="K35" s="16">
         <v>7.0</v>
       </c>
-      <c r="K35">
+      <c r="L35">
         <v>42765.0</v>
       </c>
-      <c r="L35" s="14">
+      <c r="M35" s="14">
         <v>1200.0</v>
       </c>
-      <c r="M35" s="14">
+      <c r="N35" s="14">
         <v>100.0</v>
       </c>
-      <c r="N35" s="14">
+      <c r="O35" s="14">
         <v>18.0</v>
       </c>
-      <c r="O35" s="13">
+      <c r="P35" s="13">
         <v>78.0</v>
       </c>
-      <c r="P35" s="13">
+      <c r="Q35" s="13">
         <v>360.0</v>
       </c>
-      <c r="Q35" s="15"/>
-    </row>
-    <row r="36">
+      <c r="R35" s="15"/>
+      <c r="S35" s="18"/>
+      <c r="T35" s="16"/>
+    </row>
+    <row r="36" ht="18.75">
       <c r="B36" s="12" t="s">
-        <v>63</v>
+        <v>96</v>
       </c>
       <c r="C36" s="13">
         <v>1031.0</v>
@@ -1981,32 +2326,37 @@
       <c r="I36" s="14">
         <v>2.4000000000000004</v>
       </c>
-      <c r="J36" s="15">
+      <c r="J36" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="K36" s="16">
         <v>10.0</v>
       </c>
-      <c r="K36">
+      <c r="L36">
         <v>42766.0</v>
       </c>
-      <c r="L36" s="14">
+      <c r="M36" s="14">
         <v>700.0</v>
       </c>
-      <c r="M36" s="14">
+      <c r="N36" s="14">
         <v>100.0</v>
       </c>
-      <c r="N36" s="14">
+      <c r="O36" s="14">
         <v>160.0</v>
       </c>
-      <c r="O36" s="13">
+      <c r="P36" s="13">
         <v>36.0</v>
       </c>
-      <c r="P36" s="13">
+      <c r="Q36" s="13">
         <v>740.0</v>
       </c>
-      <c r="Q36" s="15"/>
-    </row>
-    <row r="37">
+      <c r="R36" s="15"/>
+      <c r="S36" s="18"/>
+      <c r="T36" s="16"/>
+    </row>
+    <row r="37" ht="18.75">
       <c r="B37" s="12" t="s">
-        <v>64</v>
+        <v>98</v>
       </c>
       <c r="C37" s="13">
         <v>1032.0</v>
@@ -2029,32 +2379,37 @@
       <c r="I37" s="14">
         <v>9.600000000000001</v>
       </c>
-      <c r="J37" s="15">
+      <c r="J37" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="K37" s="16">
         <v>10.0</v>
       </c>
-      <c r="K37">
+      <c r="L37">
         <v>42767.0</v>
       </c>
-      <c r="L37" s="14">
+      <c r="M37" s="14">
         <v>900.0</v>
       </c>
-      <c r="M37" s="14">
+      <c r="N37" s="14">
         <v>300.0</v>
       </c>
-      <c r="N37" s="14">
+      <c r="O37" s="14">
         <v>198.0</v>
       </c>
-      <c r="O37" s="13">
+      <c r="P37" s="13">
         <v>81.0</v>
       </c>
-      <c r="P37" s="13">
+      <c r="Q37" s="13">
         <v>1320.0</v>
       </c>
-      <c r="Q37" s="15"/>
-    </row>
-    <row r="38">
+      <c r="R37" s="15"/>
+      <c r="S37" s="18"/>
+      <c r="T37" s="16"/>
+    </row>
+    <row r="38" ht="18.75">
       <c r="B38" s="12" t="s">
-        <v>65</v>
+        <v>99</v>
       </c>
       <c r="C38" s="13">
         <v>1033.0</v>
@@ -2077,34 +2432,43 @@
       <c r="I38" s="14">
         <v>3.0</v>
       </c>
-      <c r="J38" s="15">
+      <c r="J38" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="K38" s="16">
         <v>5.0</v>
       </c>
-      <c r="K38">
+      <c r="L38">
         <v>42768.0</v>
       </c>
-      <c r="L38" s="14">
+      <c r="M38" s="14">
         <v>2200.0</v>
       </c>
-      <c r="M38" s="14">
+      <c r="N38" s="14">
         <v>500.0</v>
       </c>
-      <c r="N38" s="14">
+      <c r="O38" s="14">
         <v>91.0</v>
       </c>
-      <c r="O38" s="13">
+      <c r="P38" s="13">
         <v>41.0</v>
       </c>
-      <c r="P38" s="13">
+      <c r="Q38" s="13">
         <v>1470.0</v>
       </c>
-      <c r="Q38" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="39">
+      <c r="R38" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="S38" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="T38" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" ht="18.75">
       <c r="B39" s="12" t="s">
-        <v>66</v>
+        <v>100</v>
       </c>
       <c r="C39" s="13">
         <v>1034.0</v>
@@ -2127,32 +2491,39 @@
       <c r="I39" s="14">
         <v>1.8</v>
       </c>
-      <c r="J39" s="15">
+      <c r="J39" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="K39" s="16">
         <v>10.0</v>
       </c>
-      <c r="K39">
+      <c r="L39">
         <v>42769.0</v>
       </c>
-      <c r="L39" s="14">
+      <c r="M39" s="14">
         <v>1600.0</v>
       </c>
-      <c r="M39" s="14">
+      <c r="N39" s="14">
         <v>100.0</v>
       </c>
-      <c r="N39" s="14">
+      <c r="O39" s="14">
         <v>190.0</v>
       </c>
-      <c r="O39" s="13">
+      <c r="P39" s="13">
         <v>49.0</v>
       </c>
-      <c r="P39" s="13">
+      <c r="Q39" s="13">
         <v>1060.0</v>
       </c>
-      <c r="Q39" s="15"/>
-    </row>
-    <row r="40">
+      <c r="R39" s="15"/>
+      <c r="S39" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="T39" s="16"/>
+    </row>
+    <row r="40" ht="18.75">
       <c r="B40" s="12" t="s">
-        <v>67</v>
+        <v>101</v>
       </c>
       <c r="C40" s="13">
         <v>1035.0</v>
@@ -2175,32 +2546,39 @@
       <c r="I40" s="14">
         <v>2.1</v>
       </c>
-      <c r="J40" s="15">
+      <c r="J40" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="K40" s="16">
         <v>10.0</v>
       </c>
-      <c r="K40">
+      <c r="L40">
         <v>42770.0</v>
       </c>
-      <c r="L40" s="14">
+      <c r="M40" s="14">
         <v>1800.0</v>
       </c>
-      <c r="M40" s="14">
+      <c r="N40" s="14">
         <v>300.0</v>
       </c>
-      <c r="N40" s="14">
+      <c r="O40" s="14">
         <v>167.0</v>
       </c>
-      <c r="O40" s="13">
+      <c r="P40" s="13">
         <v>97.0</v>
       </c>
-      <c r="P40" s="13">
+      <c r="Q40" s="13">
         <v>140.0</v>
       </c>
-      <c r="Q40" s="15"/>
-    </row>
-    <row r="41">
+      <c r="R40" s="15"/>
+      <c r="S40" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="T40" s="16"/>
+    </row>
+    <row r="41" ht="18.75">
       <c r="B41" s="12" t="s">
-        <v>68</v>
+        <v>102</v>
       </c>
       <c r="C41" s="13">
         <v>1036.0</v>
@@ -2223,32 +2601,39 @@
       <c r="I41" s="14">
         <v>10.200000000000001</v>
       </c>
-      <c r="J41" s="15">
+      <c r="J41" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="K41" s="16">
         <v>6.0</v>
       </c>
-      <c r="K41">
+      <c r="L41">
         <v>42771.0</v>
       </c>
-      <c r="L41" s="14">
+      <c r="M41" s="14">
         <v>500.0</v>
       </c>
-      <c r="M41" s="14">
+      <c r="N41" s="14">
         <v>400.0</v>
       </c>
-      <c r="N41" s="14">
+      <c r="O41" s="14">
         <v>115.00000000000001</v>
       </c>
-      <c r="O41" s="13">
+      <c r="P41" s="13">
         <v>38.0</v>
       </c>
-      <c r="P41" s="13">
+      <c r="Q41" s="13">
         <v>500.0</v>
       </c>
-      <c r="Q41" s="15"/>
-    </row>
-    <row r="42">
+      <c r="R41" s="15"/>
+      <c r="S41" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="T41" s="16"/>
+    </row>
+    <row r="42" ht="18.75">
       <c r="B42" s="12" t="s">
-        <v>69</v>
+        <v>104</v>
       </c>
       <c r="C42" s="13">
         <v>1037.0</v>
@@ -2271,34 +2656,43 @@
       <c r="I42" s="14">
         <v>0.4</v>
       </c>
-      <c r="J42" s="15">
+      <c r="J42" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="K42" s="16">
         <v>4.0</v>
       </c>
-      <c r="K42">
+      <c r="L42">
         <v>42772.0</v>
       </c>
-      <c r="L42" s="14">
+      <c r="M42" s="14">
         <v>1600.0</v>
       </c>
-      <c r="M42" s="14">
+      <c r="N42" s="14">
         <v>300.0</v>
       </c>
-      <c r="N42" s="14">
+      <c r="O42" s="14">
         <v>94.0</v>
       </c>
-      <c r="O42" s="13">
+      <c r="P42" s="13">
         <v>93.0</v>
       </c>
-      <c r="P42" s="13">
+      <c r="Q42" s="13">
         <v>1530.0</v>
       </c>
-      <c r="Q42" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="43">
+      <c r="R42" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="S42" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="T42" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" ht="18.75">
       <c r="B43" s="12" t="s">
-        <v>70</v>
+        <v>106</v>
       </c>
       <c r="C43" s="13">
         <v>1038.0</v>
@@ -2321,28 +2715,35 @@
       <c r="I43" s="14">
         <v>8.0</v>
       </c>
-      <c r="J43" s="15">
+      <c r="J43" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="K43" s="16">
         <v>8.0</v>
       </c>
-      <c r="K43">
+      <c r="L43">
         <v>42773.0</v>
       </c>
-      <c r="L43" s="14">
+      <c r="M43" s="14">
         <v>1200.0</v>
       </c>
-      <c r="M43" s="14">
+      <c r="N43" s="14">
         <v>500.0</v>
       </c>
-      <c r="N43" s="14">
+      <c r="O43" s="14">
         <v>66.0</v>
       </c>
-      <c r="O43" s="13">
+      <c r="P43" s="13">
         <v>51.0</v>
       </c>
-      <c r="P43" s="13">
+      <c r="Q43" s="13">
         <v>400.0</v>
       </c>
-      <c r="Q43" s="15"/>
+      <c r="R43" s="15"/>
+      <c r="S43" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="T43" s="16"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>